<commit_message>
Page Objects for Share Skill
</commit_message>
<xml_diff>
--- a/MarsFramework/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/MarsFramework/ExcelData/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t>FirstName</t>
   </si>
@@ -133,24 +133,9 @@
     <t>Tags</t>
   </si>
   <si>
-    <t>Service Type</t>
-  </si>
-  <si>
-    <t>Location Type</t>
-  </si>
-  <si>
-    <t>Skill Trade</t>
-  </si>
-  <si>
     <t>Credit</t>
   </si>
   <si>
-    <t>Skill-Exchange</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>Information</t>
   </si>
   <si>
@@ -169,15 +154,6 @@
     <t>Automation</t>
   </si>
   <si>
-    <t>One-off service</t>
-  </si>
-  <si>
-    <t>On-site</t>
-  </si>
-  <si>
-    <t>Hidden</t>
-  </si>
-  <si>
     <t>valid</t>
   </si>
   <si>
@@ -191,18 +167,6 @@
   </si>
   <si>
     <t>Video Marketing</t>
-  </si>
-  <si>
-    <t>Hourly basis service</t>
-  </si>
-  <si>
-    <t>Online</t>
-  </si>
-  <si>
-    <t>Skill-exchange</t>
-  </si>
-  <si>
-    <t>Java</t>
   </si>
   <si>
     <t>invalid</t>
@@ -213,9 +177,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
@@ -254,8 +218,114 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,131 +339,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -418,25 +382,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,157 +562,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,15 +573,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -636,17 +591,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -658,15 +602,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -704,6 +639,35 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -712,7 +676,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -730,131 +694,131 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -863,10 +827,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1256,19 +1220,19 @@
       </c>
     </row>
     <row r="2" ht="15.6" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1315,7 +1279,7 @@
       <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1387,31 +1351,31 @@
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1424,29 +1388,24 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C12" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="21.4444444444444" customWidth="1"/>
     <col min="2" max="2" width="13.8888888888889" customWidth="1"/>
     <col min="3" max="3" width="19.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="17.8888888888889" customWidth="1"/>
     <col min="5" max="5" width="16.2222222222222" customWidth="1"/>
-    <col min="6" max="6" width="21.1111111111111" customWidth="1"/>
-    <col min="7" max="7" width="16.7777777777778" customWidth="1"/>
-    <col min="8" max="8" width="15.2222222222222" customWidth="1"/>
-    <col min="9" max="9" width="12.4444444444444" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="8.33333333333333" customWidth="1"/>
-    <col min="12" max="12" width="14.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="12.4444444444444" customWidth="1"/>
+    <col min="7" max="7" width="14.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" spans="1:12">
+    <row r="1" ht="18" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1465,95 +1424,54 @@
       <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" ht="15.6" spans="1:7">
+      <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="F2" s="3">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" ht="15.6" spans="1:12">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="3" ht="15.6" spans="1:7">
+      <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="2">
-        <v>10</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" ht="15.6" spans="1:12">
-      <c r="A3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>